<commit_message>
done w LENS, SARI, FKGL
</commit_message>
<xml_diff>
--- a/src/2 models/data_output/english/out_eng_EW-SEW_LLAMA3.xlsx
+++ b/src/2 models/data_output/english/out_eng_EW-SEW_LLAMA3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_CODE\Sem4_IM\simpli-perform\src\2 models\data_output\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712B1628-33B5-44E5-8CCE-EA602806B55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7336AFDD-37C7-493A-947D-26DB6822C40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F1963640-37F6-4371-983A-88F89227F8EF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6504" uniqueCount="3109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6505" uniqueCount="3109">
   <si>
     <t>The song peaked at number six on the Billboard alternative rock chart.</t>
   </si>
@@ -9446,7 +9446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -9454,6 +9454,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9838,8 +9839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C23B16B-9475-40DD-BB60-4FAD82A439CB}">
   <dimension ref="A1:G2220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2141" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C2143" sqref="C2143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -37760,8 +37761,8 @@
       <c r="B2168" t="s">
         <v>2124</v>
       </c>
-      <c r="C2168" s="1" t="s">
-        <v>2076</v>
+      <c r="C2168" s="5" t="s">
+        <v>2065</v>
       </c>
       <c r="D2168" s="2" t="s">
         <v>3091</v>
@@ -37774,7 +37775,7 @@
       </c>
     </row>
     <row r="2169" spans="1:6">
-      <c r="C2169" s="1"/>
+      <c r="C2169" s="5"/>
     </row>
     <row r="2170" spans="1:6">
       <c r="A2170">
@@ -37783,8 +37784,8 @@
       <c r="B2170" t="s">
         <v>2125</v>
       </c>
-      <c r="C2170" s="1" t="s">
-        <v>2077</v>
+      <c r="C2170" s="5" t="s">
+        <v>2076</v>
       </c>
       <c r="D2170" s="2" t="s">
         <v>3092</v>
@@ -37797,7 +37798,7 @@
       </c>
     </row>
     <row r="2171" spans="1:6">
-      <c r="C2171" s="1"/>
+      <c r="C2171" s="5"/>
     </row>
     <row r="2172" spans="1:6">
       <c r="A2172">
@@ -37806,8 +37807,8 @@
       <c r="B2172" t="s">
         <v>2126</v>
       </c>
-      <c r="C2172" s="1" t="s">
-        <v>2078</v>
+      <c r="C2172" s="5" t="s">
+        <v>2077</v>
       </c>
       <c r="D2172" s="2" t="s">
         <v>3093</v>
@@ -37820,7 +37821,7 @@
       </c>
     </row>
     <row r="2173" spans="1:6">
-      <c r="C2173" s="1"/>
+      <c r="C2173" s="5"/>
     </row>
     <row r="2174" spans="1:6">
       <c r="A2174">
@@ -37829,8 +37830,8 @@
       <c r="B2174" t="s">
         <v>2127</v>
       </c>
-      <c r="C2174" s="1" t="s">
-        <v>2079</v>
+      <c r="C2174" s="5" t="s">
+        <v>2078</v>
       </c>
       <c r="D2174" s="2" t="s">
         <v>3094</v>
@@ -37843,7 +37844,7 @@
       </c>
     </row>
     <row r="2175" spans="1:6">
-      <c r="C2175" s="1"/>
+      <c r="C2175" s="5"/>
     </row>
     <row r="2176" spans="1:6">
       <c r="A2176">
@@ -37852,8 +37853,8 @@
       <c r="B2176" t="s">
         <v>2079</v>
       </c>
-      <c r="C2176" s="1" t="s">
-        <v>2080</v>
+      <c r="C2176" s="5" t="s">
+        <v>2079</v>
       </c>
       <c r="D2176" s="2" t="s">
         <v>3095</v>
@@ -37866,7 +37867,7 @@
       </c>
     </row>
     <row r="2177" spans="1:7">
-      <c r="C2177" s="1"/>
+      <c r="C2177" s="5"/>
     </row>
     <row r="2178" spans="1:7">
       <c r="A2178">
@@ -37875,8 +37876,8 @@
       <c r="B2178" t="s">
         <v>2128</v>
       </c>
-      <c r="C2178" s="1" t="s">
-        <v>2081</v>
+      <c r="C2178" s="5" t="s">
+        <v>2080</v>
       </c>
       <c r="D2178" s="2" t="s">
         <v>3096</v>
@@ -37889,7 +37890,7 @@
       </c>
     </row>
     <row r="2179" spans="1:7">
-      <c r="C2179" s="1"/>
+      <c r="C2179" s="5"/>
     </row>
     <row r="2180" spans="1:7">
       <c r="A2180">
@@ -37898,8 +37899,8 @@
       <c r="B2180" t="s">
         <v>2129</v>
       </c>
-      <c r="C2180" s="1" t="s">
-        <v>2082</v>
+      <c r="C2180" s="5" t="s">
+        <v>2081</v>
       </c>
       <c r="D2180" s="2" t="s">
         <v>3097</v>
@@ -37912,7 +37913,7 @@
       </c>
     </row>
     <row r="2181" spans="1:7">
-      <c r="C2181" s="1"/>
+      <c r="C2181" s="5"/>
     </row>
     <row r="2182" spans="1:7">
       <c r="A2182">
@@ -37921,8 +37922,8 @@
       <c r="B2182" t="s">
         <v>2130</v>
       </c>
-      <c r="C2182" s="1" t="s">
-        <v>2083</v>
+      <c r="C2182" s="5" t="s">
+        <v>2082</v>
       </c>
       <c r="D2182" s="2" t="s">
         <v>3098</v>
@@ -37938,7 +37939,7 @@
       </c>
     </row>
     <row r="2183" spans="1:7">
-      <c r="C2183" s="1"/>
+      <c r="C2183" s="5"/>
     </row>
     <row r="2184" spans="1:7">
       <c r="A2184">
@@ -37947,8 +37948,8 @@
       <c r="B2184" t="s">
         <v>2131</v>
       </c>
-      <c r="C2184" s="1" t="s">
-        <v>2084</v>
+      <c r="C2184" s="5" t="s">
+        <v>2083</v>
       </c>
       <c r="D2184" s="2" t="s">
         <v>3099</v>
@@ -37964,7 +37965,7 @@
       </c>
     </row>
     <row r="2185" spans="1:7">
-      <c r="C2185" s="1"/>
+      <c r="C2185" s="5"/>
     </row>
     <row r="2186" spans="1:7">
       <c r="A2186">
@@ -37973,8 +37974,8 @@
       <c r="B2186" t="s">
         <v>2132</v>
       </c>
-      <c r="C2186" s="1" t="s">
-        <v>2085</v>
+      <c r="C2186" s="5" t="s">
+        <v>2084</v>
       </c>
       <c r="D2186" s="2" t="s">
         <v>3100</v>
@@ -37990,7 +37991,7 @@
       </c>
     </row>
     <row r="2187" spans="1:7">
-      <c r="C2187" s="1"/>
+      <c r="C2187" s="5"/>
     </row>
     <row r="2188" spans="1:7">
       <c r="A2188">
@@ -37999,8 +38000,8 @@
       <c r="B2188" t="s">
         <v>2133</v>
       </c>
-      <c r="C2188" s="1" t="s">
-        <v>2086</v>
+      <c r="C2188" s="5" t="s">
+        <v>2085</v>
       </c>
       <c r="D2188" s="2" t="s">
         <v>3101</v>
@@ -38016,7 +38017,7 @@
       </c>
     </row>
     <row r="2189" spans="1:7">
-      <c r="C2189" s="1"/>
+      <c r="C2189" s="5"/>
     </row>
     <row r="2190" spans="1:7">
       <c r="A2190">
@@ -38025,8 +38026,8 @@
       <c r="B2190" t="s">
         <v>2134</v>
       </c>
-      <c r="C2190" s="1" t="s">
-        <v>2087</v>
+      <c r="C2190" s="5" t="s">
+        <v>2086</v>
       </c>
       <c r="D2190" s="2" t="s">
         <v>3102</v>
@@ -38042,7 +38043,7 @@
       </c>
     </row>
     <row r="2191" spans="1:7">
-      <c r="C2191" s="1"/>
+      <c r="C2191" s="5"/>
     </row>
     <row r="2192" spans="1:7">
       <c r="A2192">
@@ -38051,8 +38052,8 @@
       <c r="B2192" t="s">
         <v>2135</v>
       </c>
-      <c r="C2192" s="1" t="s">
-        <v>2088</v>
+      <c r="C2192" s="5" t="s">
+        <v>2087</v>
       </c>
       <c r="D2192" s="2" t="s">
         <v>3103</v>
@@ -38068,7 +38069,7 @@
       </c>
     </row>
     <row r="2193" spans="1:7">
-      <c r="C2193" s="1"/>
+      <c r="C2193" s="5"/>
     </row>
     <row r="2194" spans="1:7">
       <c r="A2194">
@@ -38077,8 +38078,8 @@
       <c r="B2194" t="s">
         <v>2136</v>
       </c>
-      <c r="C2194" s="1" t="s">
-        <v>2089</v>
+      <c r="C2194" s="5" t="s">
+        <v>2088</v>
       </c>
       <c r="D2194" s="2" t="s">
         <v>3104</v>
@@ -38094,7 +38095,7 @@
       </c>
     </row>
     <row r="2195" spans="1:7">
-      <c r="C2195" s="1"/>
+      <c r="C2195" s="5"/>
     </row>
     <row r="2196" spans="1:7">
       <c r="A2196">
@@ -38103,8 +38104,8 @@
       <c r="B2196" t="s">
         <v>2137</v>
       </c>
-      <c r="C2196" s="1" t="s">
-        <v>2090</v>
+      <c r="C2196" s="5" t="s">
+        <v>2089</v>
       </c>
       <c r="D2196" s="2" t="s">
         <v>3105</v>
@@ -38120,7 +38121,7 @@
       </c>
     </row>
     <row r="2197" spans="1:7">
-      <c r="C2197" s="1"/>
+      <c r="C2197" s="5"/>
     </row>
     <row r="2198" spans="1:7">
       <c r="A2198">
@@ -38129,8 +38130,8 @@
       <c r="B2198" t="s">
         <v>2138</v>
       </c>
-      <c r="C2198" s="1" t="s">
-        <v>2091</v>
+      <c r="C2198" s="5" t="s">
+        <v>2090</v>
       </c>
       <c r="D2198" s="2" t="s">
         <v>3106</v>
@@ -38146,7 +38147,7 @@
       </c>
     </row>
     <row r="2199" spans="1:7">
-      <c r="C2199" s="1"/>
+      <c r="C2199" s="5"/>
     </row>
     <row r="2200" spans="1:7">
       <c r="A2200">
@@ -38155,7 +38156,9 @@
       <c r="B2200" t="s">
         <v>2139</v>
       </c>
-      <c r="C2200" s="1"/>
+      <c r="C2200" s="5" t="s">
+        <v>2091</v>
+      </c>
       <c r="D2200" s="2" t="s">
         <v>3107</v>
       </c>

</xml_diff>